<commit_message>
Houston & UCONN update
</commit_message>
<xml_diff>
--- a/CBB_Prescout/headshot_url.xlsx
+++ b/CBB_Prescout/headshot_url.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Scouting\prescout\Prescout\CBB_Prescout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AEA516-3C86-49A0-91D5-F85DB3847CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0E5131-992D-4233-9B0E-2935335618E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{682FBB31-4B6A-4500-900B-D1F8CE67D1FB}"/>
+    <workbookView xWindow="7480" yWindow="2190" windowWidth="10800" windowHeight="8610" xr2:uid="{682FBB31-4B6A-4500-900B-D1F8CE67D1FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
-  <si>
-    <t>Quenton Jackson</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/nba/players/full/4592829.png&amp;w=350&amp;h=254</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>Player</t>
   </si>
@@ -50,193 +44,160 @@
     <t>Team</t>
   </si>
   <si>
-    <t>Texas A&amp;M</t>
-  </si>
-  <si>
-    <t>Javonte Brown</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702024.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Henry Coleman</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432186.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Tyrece Radford</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4395685.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Wade Taylor</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4683833.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Marcus Williams</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4703400.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
     <t>Hassan Diarra</t>
   </si>
   <si>
     <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433160.png&amp;w=350&amp;h=254</t>
   </si>
   <si>
-    <t>Andre Gordon</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4431779.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Manny Obaseki</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433277.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Hayden Hefner</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433279.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Aaron Cash</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4896467.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Ethan Henderson</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4395706.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Vince Williams</t>
-  </si>
-  <si>
-    <t>VCU</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/nba/players/full/4397227.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433182.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4397228.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Jayden Nunn</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4896614.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Hason Ward</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4592495.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Marcus Tsohonis</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4592438.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>KeShawn Curry</t>
-  </si>
-  <si>
-    <t>Ace Baldwin</t>
-  </si>
-  <si>
-    <t>Levi Stockard</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4277897.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Jalen DeLoach</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432483.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Mikeal Brown-Jones</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433224.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Nicholas Kern</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4684145.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Josh Banks</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432402.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Wake Forest</t>
-  </si>
-  <si>
-    <t>Alondes Williams</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/nba/players/full/4592216.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Jake Laravia</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/nba/players/full/4592691.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4398180.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Daivien Williamson</t>
-  </si>
-  <si>
-    <t>Isaiah Mucius</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4395686.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Dallas Walton</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4066353.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Damari Monsanto</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432916.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Khadim Sy</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4065740.png&amp;w=350&amp;h=254</t>
-  </si>
-  <si>
-    <t>Cameron Hildreth</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4696316.png&amp;w=350&amp;h=254</t>
+    <t>Terrance Arceneaux</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>https://w7.pngwing.com/pngs/177/551/png-transparent-user-interface-design-computer-icons-default-stephen-salazar-graphy-user-interface-design-computer-wallpaper-sphere-thumbnail.png</t>
+  </si>
+  <si>
+    <t>Darius Bowser</t>
+  </si>
+  <si>
+    <t>Reggie Chaney</t>
+  </si>
+  <si>
+    <t>Ryan Elvin</t>
+  </si>
+  <si>
+    <t>Ja'Vier Francis</t>
+  </si>
+  <si>
+    <t>Tramon Mark</t>
+  </si>
+  <si>
+    <t>J'Wan Roberts</t>
+  </si>
+  <si>
+    <t>Marcus Sasser</t>
+  </si>
+  <si>
+    <t>Emanuel Sharp</t>
+  </si>
+  <si>
+    <t>Jamal Shead</t>
+  </si>
+  <si>
+    <t>Jarace Walker</t>
+  </si>
+  <si>
+    <t>Ramon Walker Jr.</t>
+  </si>
+  <si>
+    <t>Mylik Wilson</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4397413.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4395708.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4701204.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4684301.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432243.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433068.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432107.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432241.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4708176.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432902.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Nahiem Alleyne</t>
+  </si>
+  <si>
+    <t>Joey Calcaterra</t>
+  </si>
+  <si>
+    <t>Donovan Clingan</t>
+  </si>
+  <si>
+    <t>Yarin Hasson</t>
+  </si>
+  <si>
+    <t>Jordan Hawkins</t>
+  </si>
+  <si>
+    <t>Emmett Hendry</t>
+  </si>
+  <si>
+    <t>Andrew Hurley</t>
+  </si>
+  <si>
+    <t>Andre Jackson Jr.</t>
+  </si>
+  <si>
+    <t>Samson Johnson</t>
+  </si>
+  <si>
+    <t>Andre Johnson Jr.</t>
+  </si>
+  <si>
+    <t>Alex Karaban</t>
+  </si>
+  <si>
+    <t>Tristen Newton</t>
+  </si>
+  <si>
+    <t>Apostolos Roumoglou</t>
+  </si>
+  <si>
+    <t>Adama Sanogo</t>
+  </si>
+  <si>
+    <t>Richie Springs</t>
+  </si>
+  <si>
+    <t>UCONN</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432934.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4280214.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4683750.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702022.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432190.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4683752.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4592965.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702023.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4592905.png&amp;w=350&amp;h=254</t>
   </si>
 </sst>
 </file>
@@ -272,8 +233,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,61 +550,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864D6C91-CF92-4839-8E28-465435B9C8C9}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.08984375" customWidth="1"/>
     <col min="3" max="3" width="86.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -650,310 +612,289 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" t="s">
-        <v>55</v>
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alabama and Michigan State update
</commit_message>
<xml_diff>
--- a/CBB_Prescout/headshot_url.xlsx
+++ b/CBB_Prescout/headshot_url.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Scouting\prescout\Prescout\CBB_Prescout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11823F3-FF13-4554-BFDC-C8CD23000E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571FB0AE-B677-4D08-8920-33178287774E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7480" yWindow="2190" windowWidth="10800" windowHeight="8610" xr2:uid="{682FBB31-4B6A-4500-900B-D1F8CE67D1FB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
   <si>
     <t>Player</t>
   </si>
@@ -216,6 +216,198 @@
   </si>
   <si>
     <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105566.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Charles Bediako</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4565203.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jaden Bradley</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432737.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Nimari Burnett</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4708027.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Noah Clowney</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4712896.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Adam Cottrell</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4598102.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Rylan Griffen</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4683682.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Noah Gurley</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4280015.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Delaney Heard</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702175.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Darius Miles</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433561.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Brandon Miller</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433287.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Nick Pringle</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4703887.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jaden Quinerly</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702179.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jahvon Quinerly</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4397132.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Max Scharnowski</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105513.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Mark Sears</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4703530.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Kai Spears</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105514.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Dominick Welch</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4397221.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jaden Akins</t>
+  </si>
+  <si>
+    <t>Michigan State</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4683730.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Pierre Brooks</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4683731.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Carson Cooper</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105817.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Malik Hall</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4592693.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Joey Hauser</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4295180.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>AJ Hoggard</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432206.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Tre Holloman</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105816.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Steven Izzo</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4592692.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jaxon Kohler</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105815.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Nick Sanders</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105818.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Mady Sissoko</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433154.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Davis Smith</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702244.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Tyson Walker</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432129.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jason Whitens</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4279457.png&amp;w=350&amp;h=254</t>
   </si>
 </sst>
 </file>
@@ -568,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864D6C91-CF92-4839-8E28-465435B9C8C9}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,6 +1103,347 @@
         <v>52</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
WSU and UCLA update
</commit_message>
<xml_diff>
--- a/CBB_Prescout/headshot_url.xlsx
+++ b/CBB_Prescout/headshot_url.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Scouting\prescout\Prescout\CBB_Prescout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571FB0AE-B677-4D08-8920-33178287774E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239EB561-FB50-4D32-A376-1CFF3F5C16BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7480" yWindow="2190" windowWidth="10800" windowHeight="8610" xr2:uid="{682FBB31-4B6A-4500-900B-D1F8CE67D1FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{682FBB31-4B6A-4500-900B-D1F8CE67D1FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="191">
   <si>
     <t>Player</t>
   </si>
@@ -408,6 +408,204 @@
   </si>
   <si>
     <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4279457.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>TJ Bamba</t>
+  </si>
+  <si>
+    <t>Washington State</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4596365.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Dylan Darling</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105658.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Adrame Diongue</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105656.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Mouhamed Gueye</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4712863.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Mael Hamon-Crespin</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105654.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Kymany Houinsou</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105659.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Dishon Jackson</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432926.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Andrej Jakimovski</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702466.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Braden Korpela</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105655.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Shae Korpela</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105653.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jabe Mullins</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4701181.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Ben Olesen</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4592673.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Justin Powell</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432250.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Myles Rice</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4709133.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>DJ Rodman</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432103.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>AJ Rohosy</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105657.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Carlos Rosario</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702465.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Dylan Andrews</t>
+  </si>
+  <si>
+    <t>UCLA</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105636.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Amari Bailey</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105638.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Adem Bona</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105637.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Tyger Campbell</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4397128.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Abramo Canka</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105635.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jaylen Clark</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432247.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Logan Cremonesi</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4702456.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Mac Etienne</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4711692.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4432848.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Evan Manjikian</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105639.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Will McClendon</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4433275.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Kenneth Nwuba</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4397129.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jack Seidler</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105640.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>David Singleton</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4397131.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Russell Stong</t>
+  </si>
+  <si>
+    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/4405598.png&amp;w=350&amp;h=254</t>
+  </si>
+  <si>
+    <t>Jaime Jaquez</t>
   </si>
 </sst>
 </file>
@@ -760,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864D6C91-CF92-4839-8E28-465435B9C8C9}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1444,6 +1642,358 @@
         <v>124</v>
       </c>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>130</v>
+      </c>
+      <c r="B64" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>146</v>
+      </c>
+      <c r="B72" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" t="s">
+        <v>126</v>
+      </c>
+      <c r="C73" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" t="s">
+        <v>126</v>
+      </c>
+      <c r="C75" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>156</v>
+      </c>
+      <c r="B77" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>158</v>
+      </c>
+      <c r="B78" t="s">
+        <v>126</v>
+      </c>
+      <c r="C78" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>160</v>
+      </c>
+      <c r="B79" t="s">
+        <v>161</v>
+      </c>
+      <c r="C79" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80" t="s">
+        <v>161</v>
+      </c>
+      <c r="C80" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" t="s">
+        <v>161</v>
+      </c>
+      <c r="C82" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>173</v>
+      </c>
+      <c r="B85" t="s">
+        <v>161</v>
+      </c>
+      <c r="C85" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" t="s">
+        <v>161</v>
+      </c>
+      <c r="C86" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>190</v>
+      </c>
+      <c r="B87" t="s">
+        <v>161</v>
+      </c>
+      <c r="C87" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>178</v>
+      </c>
+      <c r="B88" t="s">
+        <v>161</v>
+      </c>
+      <c r="C88" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89" t="s">
+        <v>161</v>
+      </c>
+      <c r="C89" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>182</v>
+      </c>
+      <c r="B90" t="s">
+        <v>161</v>
+      </c>
+      <c r="C90" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>184</v>
+      </c>
+      <c r="B91" t="s">
+        <v>161</v>
+      </c>
+      <c r="C91" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>186</v>
+      </c>
+      <c r="B92" t="s">
+        <v>161</v>
+      </c>
+      <c r="C92" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>188</v>
+      </c>
+      <c r="B93" t="s">
+        <v>161</v>
+      </c>
+      <c r="C93" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
missing headshot and PPT row duplication solutions
</commit_message>
<xml_diff>
--- a/CBB_Prescout/headshot_url.xlsx
+++ b/CBB_Prescout/headshot_url.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Scouting\prescout\Prescout\CBB_Prescout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D5237A-79D0-4B9E-9121-B274085441A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8941535A-F2A7-4FA1-A7D0-EC5DCCDB004C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{682FBB31-4B6A-4500-900B-D1F8CE67D1FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="190">
   <si>
     <t>Player</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105568.png&amp;h=80&amp;w=110&amp;scale=crop</t>
-  </si>
-  <si>
-    <t>https://a.espncdn.com/combiner/i?img=/i/headshots/nophoto.png&amp;w=110&amp;h=80&amp;scale=crop</t>
   </si>
   <si>
     <t>https://a.espncdn.com/combiner/i?img=/i/headshots/mens-college-basketball/players/full/5105567.png&amp;w=350&amp;h=254</t>
@@ -942,7 +939,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -952,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864D6C91-CF92-4839-8E28-465435B9C8C9}">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1122,7 +1119,7 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
         <v>44</v>
@@ -1133,7 +1130,7 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C16" t="s">
         <v>45</v>
@@ -1144,18 +1141,16 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>190</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1166,18 +1161,16 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>190</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
@@ -1188,7 +1181,7 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>56</v>
@@ -1199,7 +1192,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
@@ -1210,7 +1203,7 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C23" t="s">
         <v>48</v>
@@ -1221,7 +1214,7 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C24" t="s">
         <v>49</v>
@@ -1232,10 +1225,10 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1243,18 +1236,16 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>190</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C27" t="s">
         <v>50</v>
@@ -1265,10 +1256,10 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1276,7 +1267,7 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -1287,7 +1278,7 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C30" t="s">
         <v>52</v>
@@ -1295,695 +1286,695 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
         <v>60</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>61</v>
-      </c>
-      <c r="C31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
         <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
         <v>65</v>
-      </c>
-      <c r="B33" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
         <v>67</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
         <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
         <v>71</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="s">
         <v>73</v>
-      </c>
-      <c r="B37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
         <v>75</v>
-      </c>
-      <c r="B38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
         <v>77</v>
-      </c>
-      <c r="B39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="s">
         <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" t="s">
         <v>81</v>
-      </c>
-      <c r="B41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
         <v>83</v>
-      </c>
-      <c r="B42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
         <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
         <v>87</v>
-      </c>
-      <c r="B44" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
         <v>89</v>
-      </c>
-      <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
         <v>91</v>
-      </c>
-      <c r="B46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
         <v>93</v>
-      </c>
-      <c r="B47" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
         <v>95</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>96</v>
-      </c>
-      <c r="C48" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" t="s">
         <v>98</v>
-      </c>
-      <c r="B49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
         <v>100</v>
-      </c>
-      <c r="B50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" t="s">
         <v>102</v>
-      </c>
-      <c r="B51" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" t="s">
         <v>104</v>
-      </c>
-      <c r="B52" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" t="s">
         <v>106</v>
-      </c>
-      <c r="B53" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" t="s">
         <v>108</v>
-      </c>
-      <c r="B54" t="s">
-        <v>96</v>
-      </c>
-      <c r="C54" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" t="s">
         <v>110</v>
-      </c>
-      <c r="B55" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" t="s">
         <v>112</v>
-      </c>
-      <c r="B56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" t="s">
         <v>114</v>
-      </c>
-      <c r="B57" t="s">
-        <v>96</v>
-      </c>
-      <c r="C57" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" t="s">
         <v>116</v>
-      </c>
-      <c r="B58" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" t="s">
         <v>118</v>
-      </c>
-      <c r="B59" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" t="s">
         <v>120</v>
-      </c>
-      <c r="B60" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" t="s">
         <v>122</v>
-      </c>
-      <c r="B61" t="s">
-        <v>96</v>
-      </c>
-      <c r="C61" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
         <v>124</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>125</v>
-      </c>
-      <c r="C62" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
         <v>127</v>
-      </c>
-      <c r="B63" t="s">
-        <v>125</v>
-      </c>
-      <c r="C63" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" t="s">
         <v>129</v>
-      </c>
-      <c r="B64" t="s">
-        <v>125</v>
-      </c>
-      <c r="C64" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" t="s">
         <v>131</v>
-      </c>
-      <c r="B65" t="s">
-        <v>125</v>
-      </c>
-      <c r="C65" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" t="s">
         <v>133</v>
-      </c>
-      <c r="B66" t="s">
-        <v>125</v>
-      </c>
-      <c r="C66" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" t="s">
         <v>135</v>
-      </c>
-      <c r="B67" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
+        <v>124</v>
+      </c>
+      <c r="C68" t="s">
         <v>137</v>
-      </c>
-      <c r="B68" t="s">
-        <v>125</v>
-      </c>
-      <c r="C68" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" t="s">
         <v>139</v>
-      </c>
-      <c r="B69" t="s">
-        <v>125</v>
-      </c>
-      <c r="C69" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s">
         <v>141</v>
-      </c>
-      <c r="B70" t="s">
-        <v>125</v>
-      </c>
-      <c r="C70" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" t="s">
         <v>143</v>
-      </c>
-      <c r="B71" t="s">
-        <v>125</v>
-      </c>
-      <c r="C71" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" t="s">
         <v>145</v>
-      </c>
-      <c r="B72" t="s">
-        <v>125</v>
-      </c>
-      <c r="C72" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" t="s">
         <v>147</v>
-      </c>
-      <c r="B73" t="s">
-        <v>125</v>
-      </c>
-      <c r="C73" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" t="s">
         <v>149</v>
-      </c>
-      <c r="B74" t="s">
-        <v>125</v>
-      </c>
-      <c r="C74" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75" t="s">
         <v>151</v>
-      </c>
-      <c r="B75" t="s">
-        <v>125</v>
-      </c>
-      <c r="C75" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" t="s">
         <v>153</v>
-      </c>
-      <c r="B76" t="s">
-        <v>125</v>
-      </c>
-      <c r="C76" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>124</v>
+      </c>
+      <c r="C77" t="s">
         <v>155</v>
-      </c>
-      <c r="B77" t="s">
-        <v>125</v>
-      </c>
-      <c r="C77" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" t="s">
         <v>157</v>
-      </c>
-      <c r="B78" t="s">
-        <v>125</v>
-      </c>
-      <c r="C78" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>158</v>
+      </c>
+      <c r="B79" t="s">
         <v>159</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>160</v>
-      </c>
-      <c r="C79" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+      <c r="C80" t="s">
         <v>162</v>
-      </c>
-      <c r="B80" t="s">
-        <v>160</v>
-      </c>
-      <c r="C80" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>163</v>
+      </c>
+      <c r="B81" t="s">
+        <v>159</v>
+      </c>
+      <c r="C81" t="s">
         <v>164</v>
-      </c>
-      <c r="B81" t="s">
-        <v>160</v>
-      </c>
-      <c r="C81" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" t="s">
         <v>166</v>
-      </c>
-      <c r="B82" t="s">
-        <v>160</v>
-      </c>
-      <c r="C82" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" t="s">
         <v>168</v>
-      </c>
-      <c r="B83" t="s">
-        <v>160</v>
-      </c>
-      <c r="C83" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" t="s">
+        <v>159</v>
+      </c>
+      <c r="C84" t="s">
         <v>170</v>
-      </c>
-      <c r="B84" t="s">
-        <v>160</v>
-      </c>
-      <c r="C84" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" t="s">
         <v>172</v>
-      </c>
-      <c r="B85" t="s">
-        <v>160</v>
-      </c>
-      <c r="C85" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" t="s">
+        <v>159</v>
+      </c>
+      <c r="C86" t="s">
         <v>174</v>
-      </c>
-      <c r="B86" t="s">
-        <v>160</v>
-      </c>
-      <c r="C86" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C87" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" t="s">
+        <v>159</v>
+      </c>
+      <c r="C88" t="s">
         <v>177</v>
-      </c>
-      <c r="B88" t="s">
-        <v>160</v>
-      </c>
-      <c r="C88" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>178</v>
+      </c>
+      <c r="B89" t="s">
+        <v>159</v>
+      </c>
+      <c r="C89" t="s">
         <v>179</v>
-      </c>
-      <c r="B89" t="s">
-        <v>160</v>
-      </c>
-      <c r="C89" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>180</v>
+      </c>
+      <c r="B90" t="s">
+        <v>159</v>
+      </c>
+      <c r="C90" t="s">
         <v>181</v>
-      </c>
-      <c r="B90" t="s">
-        <v>160</v>
-      </c>
-      <c r="C90" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" t="s">
+        <v>159</v>
+      </c>
+      <c r="C91" t="s">
         <v>183</v>
-      </c>
-      <c r="B91" t="s">
-        <v>160</v>
-      </c>
-      <c r="C91" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>184</v>
+      </c>
+      <c r="B92" t="s">
+        <v>159</v>
+      </c>
+      <c r="C92" t="s">
         <v>185</v>
-      </c>
-      <c r="B92" t="s">
-        <v>160</v>
-      </c>
-      <c r="C92" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>186</v>
+      </c>
+      <c r="B93" t="s">
+        <v>159</v>
+      </c>
+      <c r="C93" t="s">
         <v>187</v>
-      </c>
-      <c r="B93" t="s">
-        <v>160</v>
-      </c>
-      <c r="C93" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>